<commit_message>
changed staffing levels script and uploaded new data for simulation comparison
</commit_message>
<xml_diff>
--- a/Supporting_Documents/facility info.xlsx
+++ b/Supporting_Documents/facility info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellieodole/Desktop/CompEpi/Supporting_Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eodole/Desktop/CompEpi/Supporting_Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5DA6AA9-FD7B-7040-97CC-E8B9D4DE6C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C503886-D861-4C4B-B3B8-0F07D978A686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11220" yWindow="500" windowWidth="17200" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13620" yWindow="500" windowWidth="14800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="facilities" sheetId="1" r:id="rId1"/>
@@ -717,7 +717,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H26" totalsRowShown="0">
   <autoFilter ref="A1:H26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H26">
-    <sortCondition ref="H1:H26"/>
+    <sortCondition ref="A1:A26"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="#fid"/>
@@ -1032,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1107,28 +1107,25 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>27</v>
       </c>
       <c r="K2" t="s">
         <v>1</v>
@@ -1163,7 +1160,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -1172,19 +1169,19 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K3" t="s">
         <v>2</v>
@@ -1219,16 +1216,16 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -1236,11 +1233,11 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
-      <c r="G4">
-        <v>1</v>
+      <c r="G4" t="s">
+        <v>7</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="K4" t="s">
         <v>3</v>
@@ -1275,28 +1272,28 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s">
         <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="K5" t="s">
         <v>36</v>
@@ -1331,10 +1328,10 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -1346,21 +1343,21 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
         <v>7</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
@@ -1372,13 +1369,13 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K7" t="s">
         <v>45</v>
@@ -1398,10 +1395,10 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -1419,7 +1416,7 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="K8" t="s">
         <v>46</v>
@@ -1439,10 +1436,10 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -1454,18 +1451,18 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
@@ -1474,33 +1471,33 @@
         <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
         <v>7</v>
       </c>
       <c r="H10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -1508,16 +1505,16 @@
       <c r="F11" t="s">
         <v>13</v>
       </c>
-      <c r="G11" t="s">
-        <v>7</v>
+      <c r="G11">
+        <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -1532,10 +1529,10 @@
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
       </c>
       <c r="H12" t="s">
         <v>31</v>
@@ -1543,42 +1540,42 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G13" t="s">
         <v>7</v>
       </c>
       <c r="H13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -1590,93 +1587,90 @@
         <v>1</v>
       </c>
       <c r="H14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15" t="s">
-        <v>31</v>
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" t="s">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
       </c>
       <c r="H16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G17" t="s">
         <v>7</v>
       </c>
       <c r="H17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
@@ -1688,24 +1682,24 @@
         <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" t="s">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
       </c>
       <c r="H18" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
@@ -1720,7 +1714,7 @@
         <v>7</v>
       </c>
       <c r="H19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1751,10 +1745,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
         <v>10</v>
@@ -1766,85 +1760,91 @@
         <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G21" t="s">
         <v>7</v>
       </c>
       <c r="H21" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
         <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G22" t="s">
         <v>7</v>
       </c>
       <c r="H22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E23" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="G23" t="s">
         <v>7</v>
+      </c>
+      <c r="H23" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G24" t="s">
         <v>7</v>
+      </c>
+      <c r="H24" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>